<commit_message>
new updates and readme
</commit_message>
<xml_diff>
--- a/date_hour.xlsx
+++ b/date_hour.xlsx
@@ -68,7 +68,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
@@ -448,126 +451,88 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="260" zoomScaleNormal="260" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
-    <col width="10.64" customWidth="1" style="2" min="2" max="2"/>
-    <col width="18.57" customWidth="1" style="2" min="4" max="4"/>
+    <col width="10.64" customWidth="1" style="3" min="2" max="2"/>
+    <col width="18.57" customWidth="1" style="3" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="3">
-      <c r="A1" s="2" t="inlineStr">
+    <row r="1" ht="13.8" customHeight="1" s="4">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>No.</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>Hour</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Epoch</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="13.8" customHeight="1" s="3">
-      <c r="A2" s="2" t="inlineStr">
+    <row r="2" ht="13.8" customHeight="1" s="4">
+      <c r="A2" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>13:27:09</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>20-09-22</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>1663669629.828427</v>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>09:58:27</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>21-09-22</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1663743507.768512</v>
       </c>
     </row>
-    <row r="3" ht="13.8" customHeight="1" s="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>13:27:17</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>20-09-22</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>1663669637.66614</v>
-      </c>
-    </row>
-    <row r="4" ht="13.8" customHeight="1" s="3">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>13:27:26</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>20-09-22</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1663669646.232369</v>
-      </c>
-    </row>
-    <row r="5" ht="13.8" customHeight="1" s="3"/>
-    <row r="6" ht="13.8" customHeight="1" s="3"/>
-    <row r="7" ht="13.8" customHeight="1" s="3"/>
-    <row r="8" ht="13.8" customHeight="1" s="3"/>
-    <row r="9" ht="13.8" customHeight="1" s="3"/>
-    <row r="10" ht="13.8" customHeight="1" s="3"/>
-    <row r="11" ht="13.8" customHeight="1" s="3"/>
-    <row r="12" ht="13.8" customHeight="1" s="3"/>
-    <row r="13" ht="13.8" customHeight="1" s="3"/>
-    <row r="14" ht="13.8" customHeight="1" s="3"/>
-    <row r="15" ht="13.8" customHeight="1" s="3"/>
-    <row r="16" ht="13.8" customHeight="1" s="3"/>
-    <row r="17" ht="13.8" customHeight="1" s="3"/>
-    <row r="18" ht="13.8" customHeight="1" s="3"/>
-    <row r="19" ht="13.8" customHeight="1" s="3"/>
-    <row r="20" ht="13.8" customHeight="1" s="3"/>
-    <row r="21" ht="13.8" customHeight="1" s="3"/>
-    <row r="22" ht="13.8" customHeight="1" s="3"/>
-    <row r="23" ht="13.8" customHeight="1" s="3"/>
-    <row r="24" ht="13.8" customHeight="1" s="3"/>
-    <row r="25" ht="13.8" customHeight="1" s="3"/>
-    <row r="26" ht="13.8" customHeight="1" s="3"/>
-    <row r="27" ht="13.8" customHeight="1" s="3"/>
-    <row r="28" ht="13.8" customHeight="1" s="3"/>
-    <row r="29" ht="13.8" customHeight="1" s="3"/>
-    <row r="30" ht="13.8" customHeight="1" s="3"/>
+    <row r="3" ht="13.8" customHeight="1" s="4"/>
+    <row r="4" ht="13.8" customHeight="1" s="4"/>
+    <row r="5" ht="13.8" customHeight="1" s="4"/>
+    <row r="6" ht="13.8" customHeight="1" s="4"/>
+    <row r="7" ht="13.8" customHeight="1" s="4"/>
+    <row r="8" ht="13.8" customHeight="1" s="4"/>
+    <row r="9" ht="13.8" customHeight="1" s="4"/>
+    <row r="10" ht="13.8" customHeight="1" s="4"/>
+    <row r="11" ht="13.8" customHeight="1" s="4"/>
+    <row r="12" ht="13.8" customHeight="1" s="4"/>
+    <row r="13" ht="13.8" customHeight="1" s="4"/>
+    <row r="14" ht="13.8" customHeight="1" s="4"/>
+    <row r="15" ht="13.8" customHeight="1" s="4"/>
+    <row r="16" ht="13.8" customHeight="1" s="4"/>
+    <row r="17" ht="13.8" customHeight="1" s="4"/>
+    <row r="18" ht="13.8" customHeight="1" s="4"/>
+    <row r="19" ht="13.8" customHeight="1" s="4"/>
+    <row r="20" ht="13.8" customHeight="1" s="4"/>
+    <row r="21" ht="13.8" customHeight="1" s="4"/>
+    <row r="22" ht="13.8" customHeight="1" s="4"/>
+    <row r="23" ht="13.8" customHeight="1" s="4"/>
+    <row r="24" ht="13.8" customHeight="1" s="4"/>
+    <row r="25" ht="13.8" customHeight="1" s="4"/>
+    <row r="26" ht="13.8" customHeight="1" s="4"/>
+    <row r="27" ht="13.8" customHeight="1" s="4"/>
+    <row r="28" ht="13.8" customHeight="1" s="4"/>
+    <row r="29" ht="13.8" customHeight="1" s="4"/>
+    <row r="30" ht="13.8" customHeight="1" s="4"/>
   </sheetData>
   <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
load file text-bug fixed
</commit_message>
<xml_diff>
--- a/date_hour.xlsx
+++ b/date_hour.xlsx
@@ -490,16 +490,16 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>15:52:48</t>
+          <t>21:05:41</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>05-10-22</t>
+          <t>06-10-22</t>
         </is>
       </c>
       <c r="D2" s="2" t="n">
-        <v>1664974368.494132</v>
+        <v>1665079541.348835</v>
       </c>
     </row>
     <row r="3" ht="13.8" customHeight="1" s="3">
@@ -510,16 +510,16 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15:52:53</t>
+          <t>21:05:46</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>05-10-22</t>
+          <t>06-10-22</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1664974373.919378</v>
+        <v>1665079546.478611</v>
       </c>
     </row>
     <row r="4" ht="13.8" customHeight="1" s="3"/>

</xml_diff>